<commit_message>
clean up, started work on estimate_assemblies
</commit_message>
<xml_diff>
--- a/server/migrations/TableDesign.xlsx
+++ b/server/migrations/TableDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwright\dev\est\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwright\dev\est\server\migrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE3076F-33D2-4770-85BE-597A13DA0CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458BA7F-D596-4275-B4C2-936425391DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="1830" windowWidth="22815" windowHeight="16905" xr2:uid="{6F7F5ED1-9578-4864-818C-119B76125F97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{6F7F5ED1-9578-4864-818C-119B76125F97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>12/2 BX</t>
   </si>
@@ -88,13 +88,43 @@
   </si>
   <si>
     <t>item labour</t>
+  </si>
+  <si>
+    <t>When I</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>Add assembly to estimate</t>
+  </si>
+  <si>
+    <t>SELECT ea.quantity, i.id, ai.quantity</t>
+  </si>
+  <si>
+    <t>FROM estimate e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         INNER JOIN estimate_assemblies ea on e.id = ea.estimate_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         INNER JOIN assembly a on a.id = ea.assembly_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         INNER JOIN assembly_items ai on ai.assembly_id = a.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         INNER JOIN item i on i.id = ai.item_id</t>
+  </si>
+  <si>
+    <t>WHERE e.id = '00000000-0000-0000-0000-000000000001';</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +137,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono Medium"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -135,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,11 +187,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -165,6 +218,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,56 +537,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCE24D1-8929-429F-B74D-B09EE489BFBB}">
-  <dimension ref="E18:L37"/>
+  <dimension ref="B16:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" customWidth="1"/>
+    <col min="15" max="15" width="82.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="3" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I22" t="s">
+      <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="J22" t="s">
+      <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="K22" t="s">
+      <c r="H20" t="s">
         <v>16</v>
       </c>
-      <c r="L22" t="s">
+      <c r="I20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>100</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E23" s="2">
         <v>1</v>
       </c>
@@ -537,166 +656,152 @@
         <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="2">
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
         <v>100</v>
       </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-      <c r="J23" s="2" t="s">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="2" t="s">
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
         <v>4</v>
       </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="2">
+      <c r="G28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <v>3</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="2">
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
-        <v>3</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <v>3</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
-      <c r="I26" s="2">
-        <v>4</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2">
-        <v>100</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2">
-        <v>5</v>
-      </c>
-      <c r="I28" s="2">
-        <v>2</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>5</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="7">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" s="7">
-        <v>1</v>
-      </c>
-      <c r="I30" s="7">
-        <v>4</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" t="s">
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change all decimals to int of cents
</commit_message>
<xml_diff>
--- a/server/migrations/TableDesign.xlsx
+++ b/server/migrations/TableDesign.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwright\dev\est\server\migrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458BA7F-D596-4275-B4C2-936425391DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EC2585-F94F-4A09-8611-C34330EE6BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{6F7F5ED1-9578-4864-818C-119B76125F97}"/>
+    <workbookView xWindow="2310" yWindow="2655" windowWidth="16275" windowHeight="15810" activeTab="1" xr2:uid="{6F7F5ED1-9578-4864-818C-119B76125F97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>12/2 BX</t>
   </si>
@@ -118,13 +119,28 @@
   </si>
   <si>
     <t>WHERE e.id = '00000000-0000-0000-0000-000000000001';</t>
+  </si>
+  <si>
+    <t>estimate_id</t>
+  </si>
+  <si>
+    <t>assembly_id</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>assembly_quantity</t>
+  </si>
+  <si>
+    <t>item_quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +168,15 @@
       <name val="JetBrains Mono Medium"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +198,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -222,6 +275,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCE24D1-8929-429F-B74D-B09EE489BFBB}">
   <dimension ref="B16:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -804,4 +881,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2D1338-C095-437F-A1E5-985C949521FC}">
+  <dimension ref="E4:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2</v>
+      </c>
+      <c r="H6" s="14">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="15">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
+      <c r="H9" s="16">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>